<commit_message>
IP_calculation_order_number.py without comments in the beginning. Main_file.xlsx with column 'order number'
</commit_message>
<xml_diff>
--- a/IP_calculation_Pro/Main_file.xlsx
+++ b/IP_calculation_Pro/Main_file.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1887,7 +1887,118 @@
         <v>10</v>
       </c>
       <c r="I39" s="2" t="n">
-        <v>45521.98183673737</v>
+        <v>45521.98183673611</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Коммутатор</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>ПРГС.465000.028</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>975</v>
+      </c>
+      <c r="E40" t="n">
+        <v>984</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>10.8.15.6</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>10.8.15.15</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>10</v>
+      </c>
+      <c r="I40" s="2" t="n">
+        <v>45581.50276196759</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Монитор</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>ПРГС.465000.012</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>1025</v>
+      </c>
+      <c r="E41" t="n">
+        <v>1034</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>10.8.99.0</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>10.8.99.9</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>10</v>
+      </c>
+      <c r="I41" s="2" t="n">
+        <v>45581.54614268518</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Монитор</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>ПРГС.465000.012</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>1035</v>
+      </c>
+      <c r="E42" t="n">
+        <v>1044</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>10.8.99.10</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>10.8.99.19</t>
+        </is>
+      </c>
+      <c r="H42" t="n">
+        <v>10</v>
+      </c>
+      <c r="I42" s="2" t="n">
+        <v>45581.54656073602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
program.py updated for adding to gui
</commit_message>
<xml_diff>
--- a/IP_calculation_Pro/Main_file.xlsx
+++ b/IP_calculation_Pro/Main_file.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1887,7 +1887,44 @@
         <v>10</v>
       </c>
       <c r="I39" s="2" t="n">
-        <v>45521.98183673737</v>
+        <v>45521.98183673611</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Блок управления камерами</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>ТТСК.465000.180</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>2829</v>
+      </c>
+      <c r="E40" t="n">
+        <v>2883</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>10.8.187.0</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>10.8.187.54</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>55</v>
+      </c>
+      <c r="I40" s="2" t="n">
+        <v>45583.77440717899</v>
       </c>
     </row>
   </sheetData>

</xml_diff>